<commit_message>
Cambios visuales de logos y templates, y ajuste del reporte de sistematización según solicitudes del 5 de septiembre de 2018
</commit_message>
<xml_diff>
--- a/plantillaHPV/candidatos.xlsx
+++ b/plantillaHPV/candidatos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Hpv\plantillaHPV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\HPV2018\plantillaHPV\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -109,20 +109,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>723413</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>70556</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1"/>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -141,8 +141,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2905125" y="57150"/>
-          <a:ext cx="7571888" cy="823031"/>
+          <a:off x="1409700" y="28575"/>
+          <a:ext cx="10058400" cy="914400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -479,7 +479,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>